<commit_message>
added ALL standard excel file
</commit_message>
<xml_diff>
--- a/Content/data.xlsx
+++ b/Content/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luke wang\learngit\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BDBD6B-DA31-4D11-A948-F658DEDCE1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45895F52-F6F6-4C7B-BEDD-80CBB3B933CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3390" yWindow="1740" windowWidth="18930" windowHeight="10845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3390" yWindow="1740" windowWidth="18930" windowHeight="10845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>geeks.com</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -43,10 +43,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Fun</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2+1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -60,6 +56,13 @@
   </si>
   <si>
     <t>@</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>asd</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -401,18 +404,18 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C1">
-        <v>1</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>23</v>
+      <c r="B2" t="s">
+        <v>8</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -423,10 +426,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -434,10 +437,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>